<commit_message>
Finished section 1 and did cleanup
</commit_message>
<xml_diff>
--- a/Lab2/convolution and morphology calculations.xlsx
+++ b/Lab2/convolution and morphology calculations.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="9280" yWindow="500" windowWidth="17740" windowHeight="16000" tabRatio="500"/>
+    <workbookView xWindow="4220" yWindow="560" windowWidth="19800" windowHeight="16000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,12 +19,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="4">
   <si>
     <t>Problem 3. Convolution</t>
   </si>
   <si>
-    <t>Row/Col</t>
+    <t>Problem 4. Erosion</t>
+  </si>
+  <si>
+    <t>===&gt;</t>
+  </si>
+  <si>
+    <t>Problem 4. Dilation</t>
   </si>
 </sst>
 </file>
@@ -64,7 +70,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -74,6 +80,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -87,7 +99,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="39">
+  <cellStyleXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -127,16 +139,47 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="39">
+  <cellStyles count="59">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -156,6 +199,16 @@
     <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -175,6 +228,16 @@
     <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -504,272 +567,1366 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:U29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S34" sqref="S34"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="8" width="5.33203125" customWidth="1"/>
+    <col min="9" max="9" width="2.1640625" customWidth="1"/>
+    <col min="10" max="21" width="5.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:8">
-      <c r="A1" s="3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
-      <c r="A2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1">
-        <v>1</v>
-      </c>
-      <c r="C2" s="1">
+    <row r="1" spans="1:21">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21">
+      <c r="A2" s="3"/>
+      <c r="B2" s="3">
+        <v>1</v>
+      </c>
+      <c r="C2" s="3">
         <v>2</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D2" s="3">
         <v>3</v>
       </c>
-      <c r="E2" s="1">
+      <c r="E2" s="3">
         <v>4</v>
       </c>
-      <c r="F2" s="1">
+      <c r="F2" s="3">
         <v>5</v>
       </c>
-      <c r="G2" s="1">
+      <c r="G2" s="3">
         <v>6</v>
       </c>
-      <c r="H2" s="1">
+      <c r="H2" s="3">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="A3" s="1">
-        <v>1</v>
-      </c>
-      <c r="B3">
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
+      <c r="P2" s="2"/>
+      <c r="Q2" s="2"/>
+      <c r="R2" s="2"/>
+      <c r="S2" s="2"/>
+      <c r="T2" s="2"/>
+      <c r="U2" s="2"/>
+    </row>
+    <row r="3" spans="1:21">
+      <c r="A3" s="3">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2">
         <f>(1*9+2*10+1*1)+(1*1+-4*10+1*4)+(1*9+2*2+1*9)</f>
         <v>17</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="2">
         <f>(1*9+2*10+1*1)+(1*1+-4*10+1*4)+(1*9+2*2+1*9)</f>
         <v>17</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="2">
         <f>(1*10+2*1+1*8)+(1*10+-4*4+1*9)+(1*2+2*9+1*7)</f>
         <v>50</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="2">
         <f>(1*1+2*8+1*2)+(1*4+-4*9+1*7)+(1*9+2*7+1*0)</f>
         <v>17</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="2">
         <f>(1*8+2*2+1*7)+(1*9+-4*7+1*3)+(1*7+2*0+1*10)</f>
         <v>20</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="2">
         <f>(1*2+2*7+1*8)+(1*7+-4*3+1*2)+(1*0+2*10+1*5)</f>
         <v>46</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="2">
         <f>(1*2+2*7+1*8)+(1*7+-4*3+1*2)+(1*0+2*10+1*5)</f>
         <v>46</v>
       </c>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="A4" s="1">
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2"/>
+      <c r="P3" s="2"/>
+      <c r="Q3" s="2"/>
+      <c r="R3" s="2"/>
+      <c r="S3" s="2"/>
+      <c r="T3" s="2"/>
+      <c r="U3" s="2"/>
+    </row>
+    <row r="4" spans="1:21">
+      <c r="A4" s="3">
         <v>2</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="2">
         <f>(1*9+2*10+1*1)+(1*1+-4*10+1*4)+(1*9+2*2+1*9)</f>
         <v>17</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="2">
         <f>(1*9+2*10+1*1)+(1*1+-4*10+1*4)+(1*9+2*2+1*9)</f>
         <v>17</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="2">
         <f>(1*10+2*1+1*8)+(1*10+-4*4+1*9)+(1*2+2*9+1*7)</f>
         <v>50</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="2">
         <f>(1*1+2*8+1*2)+(1*4+-4*9+1*7)+(1*9+2*7+1*0)</f>
         <v>17</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="2">
         <f>(1*8+2*2+1*7)+(1*9+-4*7+1*3)+(1*7+2*0+1*10)</f>
         <v>20</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="2">
         <f>(1*2+2*7+1*8)+(1*7+-4*3+1*2)+(1*0+2*10+1*5)</f>
         <v>46</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="2">
         <f>(1*2+2*7+1*8)+(1*7+-4*3+1*2)+(1*0+2*10+1*5)</f>
         <v>46</v>
       </c>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="A5" s="1">
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+      <c r="O4" s="2"/>
+      <c r="P4" s="2"/>
+      <c r="Q4" s="2"/>
+      <c r="R4" s="2"/>
+      <c r="S4" s="2"/>
+      <c r="T4" s="2"/>
+      <c r="U4" s="2"/>
+    </row>
+    <row r="5" spans="1:21">
+      <c r="A5" s="3">
         <v>3</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="2">
         <f>(1*1+2*10+1*4)+(1*9+-4*2+1*9)+(1*6+2*10+1*8)</f>
         <v>69</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="2">
         <f>(1*1+2*10+1*4)+(1*9+-4*2+1*9)+(1*6+2*10+1*8)</f>
         <v>69</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="2">
         <f>(1*10+2*4+1*9)+(1*2+-4*9+1*7)+(1*10+2*8+1*8)</f>
         <v>34</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="2">
         <f>(1*4+2*9+1*7)+(1*9+-4*7+1*0)+(1*8+2*8+1*3)</f>
         <v>37</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="2">
         <f>(1*9+2*7+1*3)+(1*7+-4*0+1*10)+(1*8+2*3+1*0)</f>
         <v>57</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="2">
         <f>(1*7+2*3+1*2)+(1*0+-4*10+1*5)+(1*3+2*0+1*4)</f>
         <v>-13</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="2">
         <f>(1*7+2*3+1*2)+(1*0+-4*10+1*5)+(1*3+2*0+1*4)</f>
         <v>-13</v>
       </c>
-    </row>
-    <row r="6" spans="1:8">
-      <c r="A6" s="1">
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+      <c r="O5" s="2"/>
+      <c r="P5" s="2"/>
+      <c r="Q5" s="2"/>
+      <c r="R5" s="2"/>
+      <c r="S5" s="2"/>
+      <c r="T5" s="2"/>
+      <c r="U5" s="2"/>
+    </row>
+    <row r="6" spans="1:21">
+      <c r="A6" s="3">
         <v>4</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="2">
         <f>(1*9+2*2+1*9)+(1*6+-4*10+1*8)+(1*3+2*10+1*10)</f>
         <v>29</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="2">
         <f>(1*9+2*2+1*9)+(1*6+-4*10+1*8)+(1*3+2*10+1*10)</f>
         <v>29</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="2">
         <f>(1*2+2*9+1*7)+(1*10+-4*8+1*8)+(1*10+2*10+1*7)</f>
         <v>50</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="2">
         <f>(1*9+2*7+1*0)+(1*8+-4*8+1*3)+(1*10+2*7+1*0)</f>
         <v>26</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="2">
         <f>(1*7+2*0+1*10)+(1*8+-4*3+1*0)+(1*7+2*0+1*4)</f>
         <v>24</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="2">
         <f>(1*0+2*10+1*5)+(1*3+-4*0+1*4)+(1*0+2*4+1*6)</f>
         <v>46</v>
       </c>
-      <c r="H6">
+      <c r="H6" s="2">
         <f>(1*0+2*10+1*5)+(1*3+-4*0+1*4)+(1*0+2*4+1*6)</f>
         <v>46</v>
       </c>
-    </row>
-    <row r="7" spans="1:8">
-      <c r="A7" s="1">
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="2"/>
+      <c r="P6" s="2"/>
+      <c r="Q6" s="2"/>
+      <c r="R6" s="2"/>
+      <c r="S6" s="2"/>
+      <c r="T6" s="2"/>
+      <c r="U6" s="2"/>
+    </row>
+    <row r="7" spans="1:21">
+      <c r="A7" s="3">
         <v>5</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="2">
         <f>(1*6+2*10+1*8)+(1*3+-4*10+1*10)+(1*3+2*5+1*7)</f>
         <v>27</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="2">
         <f>(1*6+2*10+1*8)+(1*3+-4*10+1*10)+(1*3+2*5+1*7)</f>
         <v>27</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="2">
         <f>(1*10+2*8+1*8)+(1*10+-4*10+1*7)+(1*5+2*7+1*4)</f>
         <v>34</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="2">
         <f>(1*8+2*8+1*3)+(1*10+-4*7+1*0)+(1*7+2*4+1*1)</f>
         <v>25</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="2">
         <f>(1*8+2*3+1*0)+(1*7+-4*0+1*4)+(1*4+2*1+1*4)</f>
         <v>35</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="2">
         <f>(1*3+2*0+1*4)+(1*0+-4*4+1*6)+(1*1+2*4+1*7)</f>
         <v>13</v>
       </c>
-      <c r="H7">
+      <c r="H7" s="2">
         <f>(1*3+2*0+1*4)+(1*0+-4*4+1*6)+(1*1+2*4+1*7)</f>
         <v>13</v>
       </c>
-    </row>
-    <row r="8" spans="1:8">
-      <c r="A8" s="1">
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2"/>
+      <c r="P7" s="2"/>
+      <c r="Q7" s="2"/>
+      <c r="R7" s="2"/>
+      <c r="S7" s="2"/>
+      <c r="T7" s="2"/>
+      <c r="U7" s="2"/>
+    </row>
+    <row r="8" spans="1:21">
+      <c r="A8" s="3">
         <v>6</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="2">
         <f>(1*1+2*10+1*10)+(1*3+-4*5+1*7)+(1*5+28+1*0)</f>
         <v>54</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="2">
         <f>(1*1+2*10+1*10)+(1*3+-4*5+1*7)+(1*5+28+1*0)</f>
         <v>54</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="2">
         <f>(1*10+2*10+1*7)+(1*5+-4*7+1*4)+(1*8+2*0+1*7)</f>
         <v>33</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="2">
         <f>(1*10+2*7+1*0)+(1*7+-4*4+1*1)+(1*0+2*7+1*8)</f>
         <v>38</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="2">
         <f>(1*7+2*0+1*4)+(1*4+-4*1+1*4)+(1*7+2*8+1*8)</f>
         <v>46</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="2">
         <f>(1*0+2*4+1*6)+(1*1+-4*4+1*7)+(1*8+2*8+1*8)</f>
         <v>38</v>
       </c>
-      <c r="H8">
+      <c r="H8" s="2">
         <f>(1*0+2*4+1*6)+(1*1+-4*4+1*7)+(1*8+2*8+1*8)</f>
         <v>38</v>
       </c>
-    </row>
-    <row r="9" spans="1:8">
-      <c r="A9" s="1">
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+      <c r="O8" s="2"/>
+      <c r="P8" s="2"/>
+      <c r="Q8" s="2"/>
+      <c r="R8" s="2"/>
+      <c r="S8" s="2"/>
+      <c r="T8" s="2"/>
+      <c r="U8" s="2"/>
+    </row>
+    <row r="9" spans="1:21">
+      <c r="A9" s="3">
         <v>7</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="2">
         <f>(1*1+2*10+1*10)+(1*3+-4*5+1*7)+(1*5+28+1*0)</f>
         <v>54</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="2">
         <f>(1*1+2*10+1*10)+(1*3+-4*5+1*7)+(1*5+28+1*0)</f>
         <v>54</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="2">
         <f>(1*10+2*10+1*7)+(1*5+-4*7+1*4)+(1*8+2*0+1*7)</f>
         <v>33</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="2">
         <f>(1*10+2*7+1*0)+(1*7+-4*4+1*1)+(1*0+2*7+1*8)</f>
         <v>38</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="2">
         <f>(1*7+2*0+1*4)+(1*4+-4*1+1*4)+(1*7+2*8+1*8)</f>
         <v>46</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="2">
         <f>(1*0+2*4+1*6)+(1*1+-4*4+1*7)+(1*8+2*8+1*8)</f>
         <v>38</v>
       </c>
-      <c r="H9">
+      <c r="H9" s="2">
         <f>(1*0+2*4+1*6)+(1*1+-4*4+1*7)+(1*8+2*8+1*8)</f>
         <v>38</v>
+      </c>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
+      <c r="O9" s="2"/>
+      <c r="P9" s="2"/>
+      <c r="Q9" s="2"/>
+      <c r="R9" s="2"/>
+      <c r="S9" s="2"/>
+      <c r="T9" s="2"/>
+      <c r="U9" s="2"/>
+    </row>
+    <row r="10" spans="1:21">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="2"/>
+      <c r="M10" s="2"/>
+      <c r="N10" s="2"/>
+      <c r="O10" s="2"/>
+      <c r="P10" s="2"/>
+      <c r="Q10" s="2"/>
+      <c r="R10" s="2"/>
+      <c r="S10" s="2"/>
+      <c r="T10" s="2"/>
+      <c r="U10" s="2"/>
+    </row>
+    <row r="11" spans="1:21">
+      <c r="A11" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
+      <c r="L11" s="2"/>
+      <c r="M11" s="2"/>
+      <c r="N11" s="2"/>
+      <c r="O11" s="2"/>
+      <c r="P11" s="2"/>
+      <c r="Q11" s="2"/>
+      <c r="R11" s="2"/>
+      <c r="S11" s="2"/>
+      <c r="T11" s="2"/>
+      <c r="U11" s="2"/>
+    </row>
+    <row r="12" spans="1:21">
+      <c r="A12" s="3"/>
+      <c r="B12" s="3">
+        <v>1</v>
+      </c>
+      <c r="C12" s="3">
+        <v>2</v>
+      </c>
+      <c r="D12" s="3">
+        <v>3</v>
+      </c>
+      <c r="E12" s="3">
+        <v>4</v>
+      </c>
+      <c r="F12" s="3">
+        <v>5</v>
+      </c>
+      <c r="G12" s="3">
+        <v>6</v>
+      </c>
+      <c r="H12" s="3">
+        <v>7</v>
+      </c>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
+      <c r="M12" s="2"/>
+      <c r="N12" s="3"/>
+      <c r="O12" s="3">
+        <v>1</v>
+      </c>
+      <c r="P12" s="3">
+        <v>2</v>
+      </c>
+      <c r="Q12" s="3">
+        <v>3</v>
+      </c>
+      <c r="R12" s="3">
+        <v>4</v>
+      </c>
+      <c r="S12" s="3">
+        <v>5</v>
+      </c>
+      <c r="T12" s="3">
+        <v>6</v>
+      </c>
+      <c r="U12" s="3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21">
+      <c r="A13" s="3">
+        <v>1</v>
+      </c>
+      <c r="B13" s="2">
+        <v>1</v>
+      </c>
+      <c r="C13" s="2">
+        <v>1</v>
+      </c>
+      <c r="D13" s="2">
+        <v>0</v>
+      </c>
+      <c r="E13" s="2">
+        <v>0</v>
+      </c>
+      <c r="F13" s="2">
+        <v>0</v>
+      </c>
+      <c r="G13" s="2">
+        <v>0</v>
+      </c>
+      <c r="H13" s="2">
+        <v>0</v>
+      </c>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
+      <c r="L13" s="2"/>
+      <c r="M13" s="2"/>
+      <c r="N13" s="3">
+        <v>1</v>
+      </c>
+      <c r="O13" s="2">
+        <v>0</v>
+      </c>
+      <c r="P13" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="2">
+        <v>0</v>
+      </c>
+      <c r="R13" s="2">
+        <v>0</v>
+      </c>
+      <c r="S13" s="2">
+        <v>0</v>
+      </c>
+      <c r="T13" s="2">
+        <v>0</v>
+      </c>
+      <c r="U13" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21">
+      <c r="A14" s="3">
+        <v>2</v>
+      </c>
+      <c r="B14" s="2">
+        <v>0</v>
+      </c>
+      <c r="C14" s="2">
+        <v>1</v>
+      </c>
+      <c r="D14" s="2">
+        <v>0</v>
+      </c>
+      <c r="E14" s="2">
+        <v>1</v>
+      </c>
+      <c r="F14" s="2">
+        <v>0</v>
+      </c>
+      <c r="G14" s="2">
+        <v>0</v>
+      </c>
+      <c r="H14" s="2">
+        <v>0</v>
+      </c>
+      <c r="I14" s="2"/>
+      <c r="J14" s="4">
+        <v>0</v>
+      </c>
+      <c r="K14" s="4">
+        <v>1</v>
+      </c>
+      <c r="L14" s="4">
+        <v>0</v>
+      </c>
+      <c r="M14" s="2"/>
+      <c r="N14" s="3">
+        <v>2</v>
+      </c>
+      <c r="O14" s="2">
+        <v>0</v>
+      </c>
+      <c r="P14" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="2">
+        <v>0</v>
+      </c>
+      <c r="R14" s="2">
+        <v>0</v>
+      </c>
+      <c r="S14" s="2">
+        <v>0</v>
+      </c>
+      <c r="T14" s="2">
+        <v>0</v>
+      </c>
+      <c r="U14" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21">
+      <c r="A15" s="3">
+        <v>3</v>
+      </c>
+      <c r="B15" s="2">
+        <v>1</v>
+      </c>
+      <c r="C15" s="2">
+        <v>0</v>
+      </c>
+      <c r="D15" s="2">
+        <v>1</v>
+      </c>
+      <c r="E15" s="2">
+        <v>0</v>
+      </c>
+      <c r="F15" s="2">
+        <v>0</v>
+      </c>
+      <c r="G15" s="2">
+        <v>1</v>
+      </c>
+      <c r="H15" s="2">
+        <v>0</v>
+      </c>
+      <c r="I15" s="2"/>
+      <c r="J15" s="4">
+        <v>1</v>
+      </c>
+      <c r="K15" s="4">
+        <v>1</v>
+      </c>
+      <c r="L15" s="4">
+        <v>1</v>
+      </c>
+      <c r="M15" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="N15" s="3">
+        <v>3</v>
+      </c>
+      <c r="O15" s="2">
+        <v>0</v>
+      </c>
+      <c r="P15" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q15" s="2">
+        <v>0</v>
+      </c>
+      <c r="R15" s="2">
+        <v>0</v>
+      </c>
+      <c r="S15" s="2">
+        <v>0</v>
+      </c>
+      <c r="T15" s="2">
+        <v>0</v>
+      </c>
+      <c r="U15" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21">
+      <c r="A16" s="3">
+        <v>4</v>
+      </c>
+      <c r="B16" s="2">
+        <v>0</v>
+      </c>
+      <c r="C16" s="2">
+        <v>1</v>
+      </c>
+      <c r="D16" s="2">
+        <v>0</v>
+      </c>
+      <c r="E16" s="2">
+        <v>0</v>
+      </c>
+      <c r="F16" s="2">
+        <v>0</v>
+      </c>
+      <c r="G16" s="2">
+        <v>0</v>
+      </c>
+      <c r="H16" s="2">
+        <v>0</v>
+      </c>
+      <c r="I16" s="2"/>
+      <c r="J16" s="4">
+        <v>0</v>
+      </c>
+      <c r="K16" s="4">
+        <v>1</v>
+      </c>
+      <c r="L16" s="4">
+        <v>0</v>
+      </c>
+      <c r="M16" s="2"/>
+      <c r="N16" s="3">
+        <v>4</v>
+      </c>
+      <c r="O16" s="2">
+        <v>0</v>
+      </c>
+      <c r="P16" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q16" s="2">
+        <v>0</v>
+      </c>
+      <c r="R16" s="2">
+        <v>0</v>
+      </c>
+      <c r="S16" s="2">
+        <v>0</v>
+      </c>
+      <c r="T16" s="2">
+        <v>0</v>
+      </c>
+      <c r="U16" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21">
+      <c r="A17" s="3">
+        <v>5</v>
+      </c>
+      <c r="B17" s="2">
+        <v>0</v>
+      </c>
+      <c r="C17" s="2">
+        <v>1</v>
+      </c>
+      <c r="D17" s="2">
+        <v>1</v>
+      </c>
+      <c r="E17" s="2">
+        <v>0</v>
+      </c>
+      <c r="F17" s="2">
+        <v>0</v>
+      </c>
+      <c r="G17" s="2">
+        <v>0</v>
+      </c>
+      <c r="H17" s="2">
+        <v>0</v>
+      </c>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="2"/>
+      <c r="L17" s="2"/>
+      <c r="M17" s="2"/>
+      <c r="N17" s="3">
+        <v>5</v>
+      </c>
+      <c r="O17" s="2">
+        <v>0</v>
+      </c>
+      <c r="P17" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q17" s="2">
+        <v>0</v>
+      </c>
+      <c r="R17" s="2">
+        <v>0</v>
+      </c>
+      <c r="S17" s="2">
+        <v>0</v>
+      </c>
+      <c r="T17" s="2">
+        <v>0</v>
+      </c>
+      <c r="U17" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21">
+      <c r="A18" s="3">
+        <v>6</v>
+      </c>
+      <c r="B18" s="2">
+        <v>0</v>
+      </c>
+      <c r="C18" s="2">
+        <v>0</v>
+      </c>
+      <c r="D18" s="2">
+        <v>0</v>
+      </c>
+      <c r="E18" s="2">
+        <v>0</v>
+      </c>
+      <c r="F18" s="2">
+        <v>0</v>
+      </c>
+      <c r="G18" s="2">
+        <v>0</v>
+      </c>
+      <c r="H18" s="2">
+        <v>0</v>
+      </c>
+      <c r="I18" s="2"/>
+      <c r="J18" s="2"/>
+      <c r="K18" s="2"/>
+      <c r="L18" s="2"/>
+      <c r="M18" s="2"/>
+      <c r="N18" s="3">
+        <v>6</v>
+      </c>
+      <c r="O18" s="2">
+        <v>0</v>
+      </c>
+      <c r="P18" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q18" s="2">
+        <v>0</v>
+      </c>
+      <c r="R18" s="2">
+        <v>0</v>
+      </c>
+      <c r="S18" s="2">
+        <v>0</v>
+      </c>
+      <c r="T18" s="2">
+        <v>0</v>
+      </c>
+      <c r="U18" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21">
+      <c r="A19" s="3">
+        <v>7</v>
+      </c>
+      <c r="B19" s="2">
+        <v>0</v>
+      </c>
+      <c r="C19" s="2">
+        <v>0</v>
+      </c>
+      <c r="D19" s="2">
+        <v>0</v>
+      </c>
+      <c r="E19" s="2">
+        <v>0</v>
+      </c>
+      <c r="F19" s="2">
+        <v>0</v>
+      </c>
+      <c r="G19" s="2">
+        <v>0</v>
+      </c>
+      <c r="H19" s="2">
+        <v>0</v>
+      </c>
+      <c r="I19" s="2"/>
+      <c r="J19" s="2"/>
+      <c r="K19" s="2"/>
+      <c r="L19" s="2"/>
+      <c r="M19" s="2"/>
+      <c r="N19" s="3">
+        <v>7</v>
+      </c>
+      <c r="O19" s="2">
+        <v>0</v>
+      </c>
+      <c r="P19" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q19" s="2">
+        <v>0</v>
+      </c>
+      <c r="R19" s="2">
+        <v>0</v>
+      </c>
+      <c r="S19" s="2">
+        <v>0</v>
+      </c>
+      <c r="T19" s="2">
+        <v>0</v>
+      </c>
+      <c r="U19" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21">
+      <c r="A21" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
+      <c r="I21" s="2"/>
+      <c r="J21" s="2"/>
+      <c r="K21" s="2"/>
+      <c r="L21" s="2"/>
+      <c r="M21" s="2"/>
+      <c r="N21" s="2"/>
+      <c r="O21" s="2"/>
+      <c r="P21" s="2"/>
+      <c r="Q21" s="2"/>
+      <c r="R21" s="2"/>
+      <c r="S21" s="2"/>
+      <c r="T21" s="2"/>
+      <c r="U21" s="2"/>
+    </row>
+    <row r="22" spans="1:21">
+      <c r="A22" s="3"/>
+      <c r="B22" s="3">
+        <v>1</v>
+      </c>
+      <c r="C22" s="3">
+        <v>2</v>
+      </c>
+      <c r="D22" s="3">
+        <v>3</v>
+      </c>
+      <c r="E22" s="3">
+        <v>4</v>
+      </c>
+      <c r="F22" s="3">
+        <v>5</v>
+      </c>
+      <c r="G22" s="3">
+        <v>6</v>
+      </c>
+      <c r="H22" s="3">
+        <v>7</v>
+      </c>
+      <c r="I22" s="2"/>
+      <c r="J22" s="2"/>
+      <c r="K22" s="2"/>
+      <c r="L22" s="2"/>
+      <c r="M22" s="2"/>
+      <c r="N22" s="3"/>
+      <c r="O22" s="3">
+        <v>1</v>
+      </c>
+      <c r="P22" s="3">
+        <v>2</v>
+      </c>
+      <c r="Q22" s="3">
+        <v>3</v>
+      </c>
+      <c r="R22" s="3">
+        <v>4</v>
+      </c>
+      <c r="S22" s="3">
+        <v>5</v>
+      </c>
+      <c r="T22" s="3">
+        <v>6</v>
+      </c>
+      <c r="U22" s="3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21">
+      <c r="A23" s="3">
+        <v>1</v>
+      </c>
+      <c r="B23" s="2">
+        <v>1</v>
+      </c>
+      <c r="C23" s="2">
+        <v>1</v>
+      </c>
+      <c r="D23" s="2">
+        <v>0</v>
+      </c>
+      <c r="E23" s="2">
+        <v>0</v>
+      </c>
+      <c r="F23" s="2">
+        <v>0</v>
+      </c>
+      <c r="G23" s="2">
+        <v>0</v>
+      </c>
+      <c r="H23" s="2">
+        <v>0</v>
+      </c>
+      <c r="I23" s="2"/>
+      <c r="J23" s="2"/>
+      <c r="K23" s="2"/>
+      <c r="L23" s="2"/>
+      <c r="M23" s="2"/>
+      <c r="N23" s="3">
+        <v>1</v>
+      </c>
+      <c r="O23" s="2">
+        <v>1</v>
+      </c>
+      <c r="P23" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q23" s="2">
+        <v>1</v>
+      </c>
+      <c r="R23" s="2">
+        <v>1</v>
+      </c>
+      <c r="S23" s="2">
+        <v>1</v>
+      </c>
+      <c r="T23" s="2">
+        <v>1</v>
+      </c>
+      <c r="U23" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21">
+      <c r="A24" s="3">
+        <v>2</v>
+      </c>
+      <c r="B24" s="2">
+        <v>0</v>
+      </c>
+      <c r="C24" s="2">
+        <v>1</v>
+      </c>
+      <c r="D24" s="2">
+        <v>0</v>
+      </c>
+      <c r="E24" s="2">
+        <v>1</v>
+      </c>
+      <c r="F24" s="2">
+        <v>0</v>
+      </c>
+      <c r="G24" s="2">
+        <v>0</v>
+      </c>
+      <c r="H24" s="2">
+        <v>0</v>
+      </c>
+      <c r="I24" s="2"/>
+      <c r="J24" s="4">
+        <v>0</v>
+      </c>
+      <c r="K24" s="4">
+        <v>1</v>
+      </c>
+      <c r="L24" s="4">
+        <v>0</v>
+      </c>
+      <c r="M24" s="2"/>
+      <c r="N24" s="3">
+        <v>2</v>
+      </c>
+      <c r="O24" s="2">
+        <v>1</v>
+      </c>
+      <c r="P24" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q24" s="2">
+        <v>1</v>
+      </c>
+      <c r="R24" s="2">
+        <v>1</v>
+      </c>
+      <c r="S24" s="2">
+        <v>1</v>
+      </c>
+      <c r="T24" s="2">
+        <v>1</v>
+      </c>
+      <c r="U24" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21">
+      <c r="A25" s="3">
+        <v>3</v>
+      </c>
+      <c r="B25" s="2">
+        <v>1</v>
+      </c>
+      <c r="C25" s="2">
+        <v>0</v>
+      </c>
+      <c r="D25" s="2">
+        <v>1</v>
+      </c>
+      <c r="E25" s="2">
+        <v>0</v>
+      </c>
+      <c r="F25" s="2">
+        <v>0</v>
+      </c>
+      <c r="G25" s="2">
+        <v>1</v>
+      </c>
+      <c r="H25" s="2">
+        <v>0</v>
+      </c>
+      <c r="I25" s="2"/>
+      <c r="J25" s="4">
+        <v>1</v>
+      </c>
+      <c r="K25" s="4">
+        <v>1</v>
+      </c>
+      <c r="L25" s="4">
+        <v>1</v>
+      </c>
+      <c r="M25" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="N25" s="3">
+        <v>3</v>
+      </c>
+      <c r="O25" s="2">
+        <v>1</v>
+      </c>
+      <c r="P25" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q25" s="2">
+        <v>1</v>
+      </c>
+      <c r="R25" s="2">
+        <v>1</v>
+      </c>
+      <c r="S25" s="2">
+        <v>1</v>
+      </c>
+      <c r="T25" s="2">
+        <v>1</v>
+      </c>
+      <c r="U25" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21">
+      <c r="A26" s="3">
+        <v>4</v>
+      </c>
+      <c r="B26" s="2">
+        <v>0</v>
+      </c>
+      <c r="C26" s="2">
+        <v>1</v>
+      </c>
+      <c r="D26" s="2">
+        <v>0</v>
+      </c>
+      <c r="E26" s="2">
+        <v>0</v>
+      </c>
+      <c r="F26" s="2">
+        <v>0</v>
+      </c>
+      <c r="G26" s="2">
+        <v>0</v>
+      </c>
+      <c r="H26" s="2">
+        <v>0</v>
+      </c>
+      <c r="I26" s="2"/>
+      <c r="J26" s="4">
+        <v>0</v>
+      </c>
+      <c r="K26" s="4">
+        <v>1</v>
+      </c>
+      <c r="L26" s="4">
+        <v>0</v>
+      </c>
+      <c r="M26" s="2"/>
+      <c r="N26" s="3">
+        <v>4</v>
+      </c>
+      <c r="O26" s="2">
+        <v>1</v>
+      </c>
+      <c r="P26" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q26" s="2">
+        <v>1</v>
+      </c>
+      <c r="R26" s="2">
+        <v>1</v>
+      </c>
+      <c r="S26" s="2">
+        <v>0</v>
+      </c>
+      <c r="T26" s="2">
+        <v>1</v>
+      </c>
+      <c r="U26" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21">
+      <c r="A27" s="3">
+        <v>5</v>
+      </c>
+      <c r="B27" s="2">
+        <v>0</v>
+      </c>
+      <c r="C27" s="2">
+        <v>1</v>
+      </c>
+      <c r="D27" s="2">
+        <v>1</v>
+      </c>
+      <c r="E27" s="2">
+        <v>0</v>
+      </c>
+      <c r="F27" s="2">
+        <v>0</v>
+      </c>
+      <c r="G27" s="2">
+        <v>0</v>
+      </c>
+      <c r="H27" s="2">
+        <v>0</v>
+      </c>
+      <c r="I27" s="2"/>
+      <c r="J27" s="2"/>
+      <c r="K27" s="2"/>
+      <c r="L27" s="2"/>
+      <c r="M27" s="2"/>
+      <c r="N27" s="3">
+        <v>5</v>
+      </c>
+      <c r="O27" s="2">
+        <v>1</v>
+      </c>
+      <c r="P27" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q27" s="2">
+        <v>1</v>
+      </c>
+      <c r="R27" s="2">
+        <v>1</v>
+      </c>
+      <c r="S27" s="2">
+        <v>1</v>
+      </c>
+      <c r="T27" s="2">
+        <v>1</v>
+      </c>
+      <c r="U27" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21">
+      <c r="A28" s="3">
+        <v>6</v>
+      </c>
+      <c r="B28" s="2">
+        <v>0</v>
+      </c>
+      <c r="C28" s="2">
+        <v>0</v>
+      </c>
+      <c r="D28" s="2">
+        <v>0</v>
+      </c>
+      <c r="E28" s="2">
+        <v>0</v>
+      </c>
+      <c r="F28" s="2">
+        <v>0</v>
+      </c>
+      <c r="G28" s="2">
+        <v>0</v>
+      </c>
+      <c r="H28" s="2">
+        <v>0</v>
+      </c>
+      <c r="I28" s="2"/>
+      <c r="J28" s="2"/>
+      <c r="K28" s="2"/>
+      <c r="L28" s="2"/>
+      <c r="M28" s="2"/>
+      <c r="N28" s="3">
+        <v>6</v>
+      </c>
+      <c r="O28" s="2">
+        <v>1</v>
+      </c>
+      <c r="P28" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q28" s="2">
+        <v>1</v>
+      </c>
+      <c r="R28" s="2">
+        <v>1</v>
+      </c>
+      <c r="S28" s="2">
+        <v>0</v>
+      </c>
+      <c r="T28" s="2">
+        <v>0</v>
+      </c>
+      <c r="U28" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21">
+      <c r="A29" s="3">
+        <v>7</v>
+      </c>
+      <c r="B29" s="2">
+        <v>0</v>
+      </c>
+      <c r="C29" s="2">
+        <v>0</v>
+      </c>
+      <c r="D29" s="2">
+        <v>0</v>
+      </c>
+      <c r="E29" s="2">
+        <v>0</v>
+      </c>
+      <c r="F29" s="2">
+        <v>0</v>
+      </c>
+      <c r="G29" s="2">
+        <v>0</v>
+      </c>
+      <c r="H29" s="2">
+        <v>0</v>
+      </c>
+      <c r="I29" s="2"/>
+      <c r="J29" s="2"/>
+      <c r="K29" s="2"/>
+      <c r="L29" s="2"/>
+      <c r="M29" s="2"/>
+      <c r="N29" s="3">
+        <v>7</v>
+      </c>
+      <c r="O29" s="2">
+        <v>0</v>
+      </c>
+      <c r="P29" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q29" s="2">
+        <v>1</v>
+      </c>
+      <c r="R29" s="2">
+        <v>0</v>
+      </c>
+      <c r="S29" s="2">
+        <v>0</v>
+      </c>
+      <c r="T29" s="2">
+        <v>0</v>
+      </c>
+      <c r="U29" s="2">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>